<commit_message>
Lab 04 - first commit
</commit_message>
<xml_diff>
--- a/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
+++ b/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F91F7E-93C1-4B3D-A7BD-B3A0940FCD3D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F1FD9F-CD54-41FF-AD1F-A5E54BFEB6D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26205" yWindow="6870" windowWidth="2985" windowHeight="585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="99">
   <si>
     <t>do not print this form</t>
   </si>
@@ -328,12 +328,6 @@
   </si>
   <si>
     <t>Req02</t>
-  </si>
-  <si>
-    <t>test passed</t>
-  </si>
-  <si>
-    <t>test passed…</t>
   </si>
   <si>
     <t>Req02_TC02</t>
@@ -1517,6 +1511,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1544,12 +1544,24 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1595,18 +1607,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1616,6 +1616,21 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1628,134 +1643,113 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2216,8 +2210,8 @@
   </sheetPr>
   <dimension ref="B1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2226,12 +2220,12 @@
       <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="50" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="52"/>
+      <c r="D1" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="54"/>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="L2" s="7" t="s">
@@ -2242,33 +2236,33 @@
       <c r="O2" s="7"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="L3" s="44" t="s">
+      <c r="L3" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="45"/>
-      <c r="N3" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="48"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="50"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="49" t="s">
+      <c r="L4" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="49"/>
+      <c r="M4" s="51"/>
       <c r="N4" s="2"/>
       <c r="O4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="46">
+      <c r="P4" s="48">
         <v>231</v>
       </c>
-      <c r="Q4" s="48"/>
+      <c r="Q4" s="50"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -2304,7 +2298,7 @@
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -2356,73 +2350,73 @@
       <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="50" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="52"/>
+      <c r="D1" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="72"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="54"/>
       <c r="F6" s="29"/>
       <c r="G6" s="29"/>
-      <c r="I6" s="50" t="s">
+      <c r="I6" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="51"/>
-      <c r="O6" s="51"/>
-      <c r="Q6" s="50" t="s">
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="53"/>
+      <c r="O6" s="53"/>
+      <c r="Q6" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="R6" s="51"/>
-      <c r="S6" s="51"/>
-      <c r="T6" s="51"/>
+      <c r="R6" s="53"/>
+      <c r="S6" s="53"/>
+      <c r="T6" s="53"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
       <c r="F8" s="30"/>
       <c r="G8" s="30"/>
       <c r="I8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="Q8" s="54" t="s">
+      <c r="Q8" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="R8" s="54"/>
-      <c r="S8" s="54"/>
+      <c r="R8" s="59"/>
+      <c r="S8" s="59"/>
       <c r="T8" s="31">
         <v>5</v>
       </c>
@@ -2431,21 +2425,21 @@
       <c r="B9" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="53" t="s">
+      <c r="C9" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
       <c r="F9" s="42"/>
       <c r="G9" s="42"/>
       <c r="I9" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="54" t="s">
+      <c r="Q9" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="R9" s="54"/>
-      <c r="S9" s="54"/>
+      <c r="R9" s="59"/>
+      <c r="S9" s="59"/>
       <c r="T9" s="31">
         <v>5</v>
       </c>
@@ -2454,22 +2448,22 @@
       <c r="B10" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="58" t="s">
+      <c r="C10" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="59"/>
-      <c r="E10" s="60"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="66"/>
       <c r="F10" s="42"/>
       <c r="G10" s="42"/>
-      <c r="I10" s="61" t="s">
+      <c r="I10" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="62"/>
-      <c r="O10" s="63"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="68"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="68"/>
+      <c r="N10" s="68"/>
+      <c r="O10" s="69"/>
       <c r="Q10" s="36" t="s">
         <v>23</v>
       </c>
@@ -2485,239 +2479,232 @@
       <c r="B11" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="58" t="s">
+      <c r="C11" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="59"/>
-      <c r="E11" s="60"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="66"/>
       <c r="F11" s="42"/>
       <c r="G11" s="42"/>
-      <c r="I11" s="64"/>
-      <c r="J11" s="65"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="65"/>
-      <c r="N11" s="65"/>
-      <c r="O11" s="66"/>
+      <c r="I11" s="70"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="71"/>
+      <c r="M11" s="71"/>
+      <c r="N11" s="71"/>
+      <c r="O11" s="72"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="58" t="s">
+      <c r="C12" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="59"/>
-      <c r="E12" s="60"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="66"/>
       <c r="F12" s="42"/>
       <c r="G12" s="42"/>
-      <c r="I12" s="64"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="65"/>
-      <c r="M12" s="65"/>
-      <c r="N12" s="65"/>
-      <c r="O12" s="66"/>
+      <c r="I12" s="70"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="71"/>
+      <c r="N12" s="71"/>
+      <c r="O12" s="72"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="58" t="s">
+      <c r="C13" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="59"/>
-      <c r="E13" s="60"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="66"/>
       <c r="F13" s="42"/>
       <c r="G13" s="42"/>
-      <c r="I13" s="64"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="65"/>
-      <c r="L13" s="65"/>
-      <c r="M13" s="65"/>
-      <c r="N13" s="65"/>
-      <c r="O13" s="66"/>
-      <c r="Q13" s="50" t="s">
+      <c r="I13" s="70"/>
+      <c r="J13" s="71"/>
+      <c r="K13" s="71"/>
+      <c r="L13" s="71"/>
+      <c r="M13" s="71"/>
+      <c r="N13" s="71"/>
+      <c r="O13" s="72"/>
+      <c r="Q13" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="R13" s="51"/>
-      <c r="S13" s="51"/>
-      <c r="T13" s="51"/>
+      <c r="R13" s="53"/>
+      <c r="S13" s="53"/>
+      <c r="T13" s="53"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="58" t="s">
+      <c r="C14" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="59"/>
-      <c r="E14" s="60"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="66"/>
       <c r="F14" s="42"/>
       <c r="G14" s="42"/>
-      <c r="I14" s="64"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="65"/>
-      <c r="M14" s="65"/>
-      <c r="N14" s="65"/>
-      <c r="O14" s="66"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="71"/>
+      <c r="K14" s="71"/>
+      <c r="L14" s="71"/>
+      <c r="M14" s="71"/>
+      <c r="N14" s="71"/>
+      <c r="O14" s="72"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="I15" s="64"/>
-      <c r="J15" s="65"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="65"/>
-      <c r="M15" s="65"/>
-      <c r="N15" s="65"/>
-      <c r="O15" s="66"/>
+      <c r="I15" s="70"/>
+      <c r="J15" s="71"/>
+      <c r="K15" s="71"/>
+      <c r="L15" s="71"/>
+      <c r="M15" s="71"/>
+      <c r="N15" s="71"/>
+      <c r="O15" s="72"/>
       <c r="Q15" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="R15" s="74" t="s">
+      <c r="R15" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="S15" s="75"/>
-      <c r="T15" s="76"/>
+      <c r="S15" s="77"/>
+      <c r="T15" s="78"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="I16" s="64"/>
-      <c r="J16" s="65"/>
-      <c r="K16" s="65"/>
-      <c r="L16" s="65"/>
-      <c r="M16" s="65"/>
-      <c r="N16" s="65"/>
-      <c r="O16" s="66"/>
+      <c r="I16" s="70"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="71"/>
+      <c r="L16" s="71"/>
+      <c r="M16" s="71"/>
+      <c r="N16" s="71"/>
+      <c r="O16" s="72"/>
       <c r="Q16" s="37">
         <v>1</v>
       </c>
-      <c r="R16" s="55" t="s">
-        <v>77</v>
-      </c>
-      <c r="S16" s="56"/>
-      <c r="T16" s="57"/>
+      <c r="R16" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="S16" s="62"/>
+      <c r="T16" s="63"/>
     </row>
     <row r="17" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I17" s="64"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="65"/>
-      <c r="L17" s="65"/>
-      <c r="M17" s="65"/>
-      <c r="N17" s="65"/>
-      <c r="O17" s="66"/>
+      <c r="I17" s="70"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="71"/>
+      <c r="M17" s="71"/>
+      <c r="N17" s="71"/>
+      <c r="O17" s="72"/>
       <c r="Q17" s="37">
         <v>2</v>
       </c>
-      <c r="R17" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="S17" s="56"/>
-      <c r="T17" s="57"/>
+      <c r="R17" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="S17" s="62"/>
+      <c r="T17" s="63"/>
     </row>
     <row r="18" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I18" s="64"/>
-      <c r="J18" s="65"/>
-      <c r="K18" s="65"/>
-      <c r="L18" s="65"/>
-      <c r="M18" s="65"/>
-      <c r="N18" s="65"/>
-      <c r="O18" s="66"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="71"/>
+      <c r="K18" s="71"/>
+      <c r="L18" s="71"/>
+      <c r="M18" s="71"/>
+      <c r="N18" s="71"/>
+      <c r="O18" s="72"/>
       <c r="Q18" s="37">
         <v>3</v>
       </c>
-      <c r="R18" s="55" t="s">
-        <v>79</v>
-      </c>
-      <c r="S18" s="56"/>
-      <c r="T18" s="57"/>
+      <c r="R18" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="S18" s="62"/>
+      <c r="T18" s="63"/>
     </row>
     <row r="19" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I19" s="64"/>
-      <c r="J19" s="65"/>
-      <c r="K19" s="65"/>
-      <c r="L19" s="65"/>
-      <c r="M19" s="65"/>
-      <c r="N19" s="65"/>
-      <c r="O19" s="66"/>
+      <c r="I19" s="70"/>
+      <c r="J19" s="71"/>
+      <c r="K19" s="71"/>
+      <c r="L19" s="71"/>
+      <c r="M19" s="71"/>
+      <c r="N19" s="71"/>
+      <c r="O19" s="72"/>
       <c r="Q19" s="37">
         <v>4</v>
       </c>
-      <c r="R19" s="55" t="s">
-        <v>80</v>
-      </c>
-      <c r="S19" s="56"/>
-      <c r="T19" s="57"/>
+      <c r="R19" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="S19" s="62"/>
+      <c r="T19" s="63"/>
     </row>
     <row r="20" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I20" s="64"/>
-      <c r="J20" s="65"/>
-      <c r="K20" s="65"/>
-      <c r="L20" s="65"/>
-      <c r="M20" s="65"/>
-      <c r="N20" s="65"/>
-      <c r="O20" s="66"/>
+      <c r="I20" s="70"/>
+      <c r="J20" s="71"/>
+      <c r="K20" s="71"/>
+      <c r="L20" s="71"/>
+      <c r="M20" s="71"/>
+      <c r="N20" s="71"/>
+      <c r="O20" s="72"/>
       <c r="Q20" s="37">
         <v>5</v>
       </c>
-      <c r="R20" s="55" t="s">
-        <v>81</v>
-      </c>
-      <c r="S20" s="56"/>
-      <c r="T20" s="57"/>
+      <c r="R20" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="S20" s="62"/>
+      <c r="T20" s="63"/>
     </row>
     <row r="21" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I21" s="64"/>
-      <c r="J21" s="65"/>
-      <c r="K21" s="65"/>
-      <c r="L21" s="65"/>
-      <c r="M21" s="65"/>
-      <c r="N21" s="65"/>
-      <c r="O21" s="66"/>
+      <c r="I21" s="70"/>
+      <c r="J21" s="71"/>
+      <c r="K21" s="71"/>
+      <c r="L21" s="71"/>
+      <c r="M21" s="71"/>
+      <c r="N21" s="71"/>
+      <c r="O21" s="72"/>
       <c r="Q21" s="37">
         <v>6</v>
       </c>
-      <c r="R21" s="55" t="s">
-        <v>82</v>
-      </c>
-      <c r="S21" s="56"/>
-      <c r="T21" s="57"/>
+      <c r="R21" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="S21" s="62"/>
+      <c r="T21" s="63"/>
     </row>
     <row r="22" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I22" s="64"/>
-      <c r="J22" s="65"/>
-      <c r="K22" s="65"/>
-      <c r="L22" s="65"/>
-      <c r="M22" s="65"/>
-      <c r="N22" s="65"/>
-      <c r="O22" s="66"/>
+      <c r="I22" s="70"/>
+      <c r="J22" s="71"/>
+      <c r="K22" s="71"/>
+      <c r="L22" s="71"/>
+      <c r="M22" s="71"/>
+      <c r="N22" s="71"/>
+      <c r="O22" s="72"/>
     </row>
     <row r="23" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I23" s="64"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="65"/>
-      <c r="M23" s="65"/>
-      <c r="N23" s="65"/>
-      <c r="O23" s="66"/>
+      <c r="I23" s="70"/>
+      <c r="J23" s="71"/>
+      <c r="K23" s="71"/>
+      <c r="L23" s="71"/>
+      <c r="M23" s="71"/>
+      <c r="N23" s="71"/>
+      <c r="O23" s="72"/>
     </row>
     <row r="24" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I24" s="67"/>
-      <c r="J24" s="68"/>
-      <c r="K24" s="68"/>
-      <c r="L24" s="68"/>
-      <c r="M24" s="68"/>
-      <c r="N24" s="68"/>
-      <c r="O24" s="69"/>
+      <c r="I24" s="73"/>
+      <c r="J24" s="74"/>
+      <c r="K24" s="74"/>
+      <c r="L24" s="74"/>
+      <c r="M24" s="74"/>
+      <c r="N24" s="74"/>
+      <c r="O24" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="I6:O6"/>
-    <mergeCell ref="Q6:T6"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="Q9:S9"/>
     <mergeCell ref="R16:T16"/>
@@ -2734,6 +2721,13 @@
     <mergeCell ref="R17:T17"/>
     <mergeCell ref="R15:T15"/>
     <mergeCell ref="R19:T19"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="I6:O6"/>
+    <mergeCell ref="Q6:T6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2781,85 +2775,85 @@
       <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="52"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="54"/>
     </row>
     <row r="3" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="72"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="57"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B5" s="12"/>
     </row>
     <row r="6" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="83" t="s">
+      <c r="B6" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="83" t="s">
+      <c r="C6" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="84" t="s">
+      <c r="D6" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="83" t="s">
+      <c r="E6" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="83"/>
-      <c r="J6" s="83"/>
-      <c r="K6" s="83"/>
-      <c r="L6" s="83"/>
-      <c r="M6" s="83"/>
-      <c r="N6" s="83"/>
-      <c r="O6" s="83"/>
-      <c r="P6" s="83"/>
-      <c r="Q6" s="83"/>
-      <c r="R6" s="83"/>
-      <c r="S6" s="83"/>
-      <c r="T6" s="83"/>
-      <c r="U6" s="83"/>
-      <c r="V6" s="83"/>
-      <c r="W6" s="83"/>
-      <c r="X6" s="83"/>
-      <c r="Y6" s="83"/>
-      <c r="Z6" s="83"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="79"/>
+      <c r="N6" s="79"/>
+      <c r="O6" s="79"/>
+      <c r="P6" s="79"/>
+      <c r="Q6" s="79"/>
+      <c r="R6" s="79"/>
+      <c r="S6" s="79"/>
+      <c r="T6" s="79"/>
+      <c r="U6" s="79"/>
+      <c r="V6" s="79"/>
+      <c r="W6" s="79"/>
+      <c r="X6" s="79"/>
+      <c r="Y6" s="79"/>
+      <c r="Z6" s="79"/>
     </row>
     <row r="7" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="83"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="80" t="s">
+      <c r="B7" s="79"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="79" t="s">
+      <c r="F7" s="86" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="79"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
-      <c r="L7" s="79"/>
-      <c r="M7" s="79"/>
-      <c r="N7" s="81" t="s">
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
+      <c r="L7" s="86"/>
+      <c r="M7" s="86"/>
+      <c r="N7" s="83" t="s">
         <v>37</v>
       </c>
-      <c r="O7" s="81"/>
-      <c r="P7" s="81"/>
-      <c r="Q7" s="81"/>
-      <c r="R7" s="81"/>
-      <c r="S7" s="81"/>
+      <c r="O7" s="83"/>
+      <c r="P7" s="83"/>
+      <c r="Q7" s="83"/>
+      <c r="R7" s="83"/>
+      <c r="S7" s="83"/>
       <c r="T7" s="82" t="s">
         <v>38</v>
       </c>
@@ -2871,42 +2865,42 @@
       <c r="Z7" s="82"/>
     </row>
     <row r="8" spans="2:26" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="83"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="79" t="s">
+      <c r="B8" s="79"/>
+      <c r="C8" s="84"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="86" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="G8" s="79"/>
-      <c r="H8" s="79" t="s">
+      <c r="K8" s="86"/>
+      <c r="L8" s="86" t="s">
         <v>84</v>
       </c>
-      <c r="I8" s="79"/>
-      <c r="J8" s="79" t="s">
-        <v>85</v>
-      </c>
-      <c r="K8" s="79"/>
-      <c r="L8" s="79" t="s">
-        <v>86</v>
-      </c>
-      <c r="M8" s="79"/>
-      <c r="N8" s="81">
+      <c r="M8" s="86"/>
+      <c r="N8" s="83">
         <v>1</v>
       </c>
-      <c r="O8" s="81">
+      <c r="O8" s="83">
         <v>2</v>
       </c>
-      <c r="P8" s="81">
+      <c r="P8" s="83">
         <v>3</v>
       </c>
-      <c r="Q8" s="81">
+      <c r="Q8" s="83">
         <v>4</v>
       </c>
-      <c r="R8" s="81">
+      <c r="R8" s="83">
         <v>5</v>
       </c>
-      <c r="S8" s="81">
+      <c r="S8" s="83">
         <v>6</v>
       </c>
       <c r="T8" s="82">
@@ -2932,10 +2926,10 @@
       </c>
     </row>
     <row r="9" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="83"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="80"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="87"/>
       <c r="F9" s="38" t="s">
         <v>43</v>
       </c>
@@ -2960,12 +2954,12 @@
       <c r="M9" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="N9" s="81"/>
-      <c r="O9" s="81"/>
-      <c r="P9" s="81"/>
-      <c r="Q9" s="81"/>
-      <c r="R9" s="81"/>
-      <c r="S9" s="81"/>
+      <c r="N9" s="83"/>
+      <c r="O9" s="83"/>
+      <c r="P9" s="83"/>
+      <c r="Q9" s="83"/>
+      <c r="R9" s="83"/>
+      <c r="S9" s="83"/>
       <c r="T9" s="82"/>
       <c r="U9" s="82"/>
       <c r="V9" s="82"/>
@@ -2979,13 +2973,13 @@
         <v>45</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="17" t="s">
@@ -3031,16 +3025,16 @@
     </row>
     <row r="11" spans="2:26" ht="63" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>90</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>92</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>46</v>
@@ -3088,16 +3082,16 @@
     </row>
     <row r="12" spans="2:26" ht="63" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="121" t="s">
-        <v>91</v>
+        <v>57</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>89</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>46</v>
@@ -3170,6 +3164,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:M7"/>
+    <mergeCell ref="N7:S7"/>
+    <mergeCell ref="Z8:Z9"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B6:B9"/>
@@ -3186,19 +3193,6 @@
     <mergeCell ref="W8:W9"/>
     <mergeCell ref="R8:R9"/>
     <mergeCell ref="T7:Z7"/>
-    <mergeCell ref="Z8:Z9"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:M7"/>
-    <mergeCell ref="N7:S7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3212,8 +3206,8 @@
   </sheetPr>
   <dimension ref="B1:O17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3236,60 +3230,60 @@
       <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="52"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="54"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="100" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="107" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="114" t="s">
+      <c r="C4" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="96" t="s">
+      <c r="D4" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="98" t="s">
+      <c r="E4" s="113" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="113"/>
-      <c r="G4" s="113"/>
-      <c r="H4" s="113"/>
-      <c r="I4" s="113"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="98" t="s">
+      <c r="F4" s="117"/>
+      <c r="G4" s="117"/>
+      <c r="H4" s="117"/>
+      <c r="I4" s="117"/>
+      <c r="J4" s="114"/>
+      <c r="K4" s="113" t="s">
         <v>52</v>
       </c>
-      <c r="L4" s="90"/>
+      <c r="L4" s="114"/>
     </row>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="107"/>
-      <c r="C5" s="115"/>
-      <c r="D5" s="97"/>
+      <c r="B5" s="108"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="119"/>
       <c r="E5" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>53</v>
@@ -3302,72 +3296,72 @@
       <c r="B6" s="20">
         <v>9</v>
       </c>
-      <c r="C6" s="111" t="s">
+      <c r="C6" s="115" t="s">
         <v>55</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="123" t="s">
-        <v>99</v>
+      <c r="E6" s="45" t="s">
+        <v>97</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>57</v>
+        <v>95</v>
+      </c>
+      <c r="G6" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="21" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="20">
         <v>10</v>
       </c>
-      <c r="C7" s="111"/>
+      <c r="C7" s="115"/>
       <c r="D7" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="123" t="s">
-        <v>100</v>
+        <v>56</v>
+      </c>
+      <c r="E7" s="45" t="s">
+        <v>98</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>57</v>
+        <v>96</v>
+      </c>
+      <c r="G7" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="20" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="20">
         <v>11</v>
       </c>
-      <c r="C8" s="111"/>
+      <c r="C8" s="115"/>
       <c r="D8" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" s="123" t="s">
-        <v>100</v>
+        <v>57</v>
+      </c>
+      <c r="E8" s="45" t="s">
+        <v>98</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>57</v>
+        <v>96</v>
+      </c>
+      <c r="G8" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="20" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="20">
         <v>12</v>
       </c>
-      <c r="C9" s="111"/>
+      <c r="C9" s="115"/>
       <c r="D9" s="43" t="s">
         <v>18</v>
       </c>
@@ -3388,7 +3382,7 @@
       <c r="B10" s="4">
         <v>13</v>
       </c>
-      <c r="C10" s="112"/>
+      <c r="C10" s="116"/>
       <c r="D10" s="39" t="s">
         <v>18</v>
       </c>
@@ -3425,98 +3419,98 @@
       <c r="F12" s="22"/>
       <c r="G12" s="22"/>
       <c r="H12" s="22"/>
-      <c r="I12" s="89"/>
-      <c r="J12" s="89"/>
+      <c r="I12" s="88"/>
+      <c r="J12" s="88"/>
       <c r="K12" s="22"/>
     </row>
     <row r="13" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="K13" s="22"/>
+    </row>
+    <row r="14" spans="2:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="95" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="96"/>
+      <c r="E14" s="96"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="K13" s="22"/>
-    </row>
-    <row r="14" spans="2:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="91" t="s">
+      <c r="I14" s="95" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="92"/>
-      <c r="E14" s="92"/>
-      <c r="F14" s="92"/>
-      <c r="G14" s="93"/>
-      <c r="H14" s="8" t="s">
+      <c r="J14" s="96"/>
+      <c r="K14" s="96"/>
+      <c r="L14" s="96"/>
+      <c r="M14" s="97"/>
+      <c r="N14" s="89" t="s">
         <v>62</v>
       </c>
-      <c r="I14" s="91" t="s">
+      <c r="O14" s="90"/>
+    </row>
+    <row r="15" spans="2:15" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="111" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="120" t="s">
         <v>63</v>
       </c>
-      <c r="J14" s="92"/>
-      <c r="K14" s="92"/>
-      <c r="L14" s="92"/>
-      <c r="M14" s="93"/>
-      <c r="N14" s="116" t="s">
+      <c r="D15" s="101" t="s">
         <v>64</v>
       </c>
-      <c r="O14" s="117"/>
-    </row>
-    <row r="15" spans="2:15" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="87" t="s">
+      <c r="E15" s="101" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="100" t="s">
+      <c r="F15" s="98" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="100" t="s">
+      <c r="G15" s="109" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="119" t="s">
+      <c r="H15" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="G15" s="122" t="s">
+      <c r="I15" s="103" t="s">
         <v>69</v>
       </c>
-      <c r="H15" s="104" t="s">
+      <c r="J15" s="112" t="s">
+        <v>63</v>
+      </c>
+      <c r="K15" s="101" t="s">
+        <v>64</v>
+      </c>
+      <c r="L15" s="110" t="s">
         <v>70</v>
       </c>
-      <c r="I15" s="102" t="s">
+      <c r="M15" s="122" t="s">
+        <v>66</v>
+      </c>
+      <c r="N15" s="91" t="s">
+        <v>69</v>
+      </c>
+      <c r="O15" s="93" t="s">
         <v>71</v>
       </c>
-      <c r="J15" s="110" t="s">
-        <v>65</v>
-      </c>
-      <c r="K15" s="100" t="s">
-        <v>66</v>
-      </c>
-      <c r="L15" s="109" t="s">
-        <v>72</v>
-      </c>
-      <c r="M15" s="94" t="s">
-        <v>68</v>
-      </c>
-      <c r="N15" s="96" t="s">
-        <v>71</v>
-      </c>
-      <c r="O15" s="114" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="86"/>
-      <c r="C16" s="88"/>
-      <c r="D16" s="101"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="120"/>
-      <c r="G16" s="108"/>
-      <c r="H16" s="105"/>
-      <c r="I16" s="103"/>
-      <c r="J16" s="100"/>
-      <c r="K16" s="101"/>
-      <c r="L16" s="86"/>
-      <c r="M16" s="95"/>
-      <c r="N16" s="118"/>
-      <c r="O16" s="108"/>
+      <c r="B16" s="111"/>
+      <c r="C16" s="121"/>
+      <c r="D16" s="102"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="99"/>
+      <c r="G16" s="94"/>
+      <c r="H16" s="106"/>
+      <c r="I16" s="104"/>
+      <c r="J16" s="101"/>
+      <c r="K16" s="102"/>
+      <c r="L16" s="111"/>
+      <c r="M16" s="123"/>
+      <c r="N16" s="92"/>
+      <c r="O16" s="94"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="23" t="s">
@@ -3550,12 +3544,10 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="I14:M14"/>
+    <mergeCell ref="M15:M16"/>
     <mergeCell ref="B3:L3"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="I15:I16"/>
@@ -3572,10 +3564,12 @@
     <mergeCell ref="E4:J4"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="I14:M14"/>
-    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="F15:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>